<commit_message>
ridefinizione del json per le vie del parcheggio e rar compresso del progetto
</commit_message>
<xml_diff>
--- a/parcheggio/scheda.xlsx
+++ b/parcheggio/scheda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VM\CONDIVISI\Siti\progetti-web\parcheggio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F57CF8B-3841-4D5D-8E14-F3C0D6882765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5148F981-B24F-4196-8DD3-1CCF16F65A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{31E115FB-E066-4BFF-89FB-25F4368C3F76}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Foglio1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DatiEsterni_1" localSheetId="0" hidden="1">fileout!$A$2:$Q$5</definedName>
+    <definedName name="DatiEsterni_1" localSheetId="0" hidden="1">fileout!$A$2:$Q$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>Column10</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Pio XII</t>
+  </si>
+  <si>
+    <t>Magna Grecia</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -226,17 +229,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -366,6 +369,12 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -430,26 +439,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38D3B455-9FE5-4211-99B1-42D4365E3CAC}" name="fileout" displayName="fileout" ref="A2:Q5" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A2:Q5" xr:uid="{38D3B455-9FE5-4211-99B1-42D4365E3CAC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38D3B455-9FE5-4211-99B1-42D4365E3CAC}" name="fileout" displayName="fileout" ref="A2:Q6" tableType="queryTable" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A2:Q6" xr:uid="{38D3B455-9FE5-4211-99B1-42D4365E3CAC}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{4A653D6C-D768-408F-A722-4E4838DDDB12}" uniqueName="1" name="Colonna1" queryTableFieldId="1" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{04817038-E1A1-4D7C-934D-4DC503DA0A4B}" uniqueName="2" name="Colonna2" queryTableFieldId="2" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{001F86A5-FC47-4736-9E6F-045800349AFC}" uniqueName="3" name="Colonna3" queryTableFieldId="3" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{4E3A9EC4-FCE9-4F69-8F90-0AC5FA45B868}" uniqueName="4" name="Colonna4" queryTableFieldId="4" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{7AE8722E-4065-47F8-93C1-A2DACEE66DF4}" uniqueName="5" name="Colonna5" queryTableFieldId="5" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{6CBFAAF9-3493-4BB2-9735-64CBFA0B71F4}" uniqueName="6" name="Colonna6" queryTableFieldId="6" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{C73F308B-9D95-4868-8CA4-BAF6BC4EC5D7}" uniqueName="7" name="Colonna7" queryTableFieldId="7" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{61BAF892-C61F-4E39-8F1B-CB05D96EB924}" uniqueName="8" name="Colonna8" queryTableFieldId="8" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{657398F2-1BA1-484C-AC05-43A75F923F00}" uniqueName="9" name="Colonna9" queryTableFieldId="9" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{B427F844-AD9C-4093-A34A-3FB263F26D66}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{83ECB083-FA89-4749-B337-2C6EEC4E15A1}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{410C6425-A6AD-458B-B466-422190EA3512}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{252FA597-950C-44D8-83C9-1E5F81800B13}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{723961E9-8A5F-4AF1-AF8F-CC415BDDBB10}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{4BB7E4B8-13A5-408F-98E4-E08B81B94690}" uniqueName="15" name="Column15" queryTableFieldId="15" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{25D5686B-5185-479A-8813-4DD2C30DCF89}" uniqueName="16" name="Column16" queryTableFieldId="16" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{96247B0F-1839-4467-A27D-8D16E40FB068}" uniqueName="17" name="Column17" queryTableFieldId="17" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{4A653D6C-D768-408F-A722-4E4838DDDB12}" uniqueName="1" name="Colonna1" queryTableFieldId="1" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{04817038-E1A1-4D7C-934D-4DC503DA0A4B}" uniqueName="2" name="Colonna2" queryTableFieldId="2" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{001F86A5-FC47-4736-9E6F-045800349AFC}" uniqueName="3" name="Colonna3" queryTableFieldId="3" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{4E3A9EC4-FCE9-4F69-8F90-0AC5FA45B868}" uniqueName="4" name="Colonna4" queryTableFieldId="4" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{7AE8722E-4065-47F8-93C1-A2DACEE66DF4}" uniqueName="5" name="Colonna5" queryTableFieldId="5" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{6CBFAAF9-3493-4BB2-9735-64CBFA0B71F4}" uniqueName="6" name="Colonna6" queryTableFieldId="6" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{C73F308B-9D95-4868-8CA4-BAF6BC4EC5D7}" uniqueName="7" name="Colonna7" queryTableFieldId="7" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{61BAF892-C61F-4E39-8F1B-CB05D96EB924}" uniqueName="8" name="Colonna8" queryTableFieldId="8" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{657398F2-1BA1-484C-AC05-43A75F923F00}" uniqueName="9" name="Colonna9" queryTableFieldId="9" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{B427F844-AD9C-4093-A34A-3FB263F26D66}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{83ECB083-FA89-4749-B337-2C6EEC4E15A1}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{410C6425-A6AD-458B-B466-422190EA3512}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{252FA597-950C-44D8-83C9-1E5F81800B13}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{723961E9-8A5F-4AF1-AF8F-CC415BDDBB10}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{4BB7E4B8-13A5-408F-98E4-E08B81B94690}" uniqueName="15" name="Column15" queryTableFieldId="15" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{25D5686B-5185-479A-8813-4DD2C30DCF89}" uniqueName="16" name="Column16" queryTableFieldId="16" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{96247B0F-1839-4467-A27D-8D16E40FB068}" uniqueName="17" name="Column17" queryTableFieldId="17" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -752,25 +761,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8545DE51-31E2-48AF-8E66-8F362892CBC7}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="10.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="11.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="11.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="16384" width="13.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -987,6 +986,32 @@
       <c r="Q5" s="4" t="s">
         <v>32</v>
       </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="6"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="6"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="6"/>
+      <c r="Q6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>